<commit_message>
Integration tests have been taken care of.
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/properties-fail-required-fields.test.xlsx
+++ b/conf-core/src/test/resources/dataloader/properties-fail-required-fields.test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\dataloader-tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ess-git\ccdb\conf-core\src\test\resources\dataloader\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -127,13 +127,19 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>https://ccdb.esss.lu.se/resources/help/ccdb_conventions.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +151,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,10 +202,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -205,8 +220,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,7 +526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -530,7 +547,7 @@
         <v>15</v>
       </c>
       <c r="E1">
-        <f xml:space="preserve"> SUMPRODUCT((B9:B65536 &lt;&gt; "") / COUNTIF(B9:B65536, B9:B65536 &amp; ""))</f>
+        <f xml:space="preserve"> SUMPRODUCT((B10:B65537 &lt;&gt; "") / COUNTIF(B10:B65537, B10:B65537 &amp; ""))</f>
         <v>4</v>
       </c>
     </row>
@@ -545,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <f xml:space="preserve"> COUNTIF(A8:A65536, "CREATE")</f>
+        <f xml:space="preserve"> COUNTIF(A9:A65537, "CREATE")</f>
         <v>5</v>
       </c>
     </row>
@@ -560,7 +577,7 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <f xml:space="preserve"> COUNTIF(A8:A65536, "UPDATE")</f>
+        <f xml:space="preserve"> COUNTIF(A9:A65537, "UPDATE")</f>
         <v>0</v>
       </c>
     </row>
@@ -575,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <f xml:space="preserve"> COUNTIF(A8:A65536, "DELETE")</f>
+        <f xml:space="preserve"> COUNTIF(A9:A65537, "DELETE")</f>
         <v>0</v>
       </c>
     </row>
@@ -595,53 +612,43 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="7" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="D10" s="6" t="s">
         <v>25</v>
       </c>
@@ -657,15 +664,15 @@
         <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>35</v>
       </c>
@@ -675,66 +682,87 @@
         <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="A8:F8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14:A1048576">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="A9:F9"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A15:A1048576">
       <formula1>"CREATE,UPDATE,DELETE"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The unit name must be between 1 and 32 characters long." sqref="E9:E13">
+    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The unit name must be between 1 and 32 characters long." sqref="E10:E14">
       <formula1>1</formula1>
       <formula2>32</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The data type name must be between 1 and 64 characters long." sqref="D9:D13">
+    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The data type name must be between 1 and 64 characters long." sqref="D10:D14">
       <formula1>1</formula1>
       <formula2>64</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The property description must be between 1 and 64 characters long." sqref="C9:C13">
+    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The property description must be between 1 and 64 characters long." sqref="C10:C14">
       <formula1>1</formula1>
       <formula2>255</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The property name must be between 1 and 64 characters long." sqref="B9:B13">
+    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The property name must be between 1 and 64 characters long." sqref="B10:B14">
       <formula1>1</formula1>
       <formula2>64</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:A14">
       <formula1>"CREATE,UPDATE,DELETE,END"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F1048576">
       <formula1>"NONE,TYPE,UNIVERSAL"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <ignoredErrors>
     <ignoredError sqref="B2" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>